<commit_message>
creacion de los csv postpandemia
</commit_message>
<xml_diff>
--- a/raw_data/raw_data_post_pan/10_1_Vistas_2-6.xlsx
+++ b/raw_data/raw_data_post_pan/10_1_Vistas_2-6.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iteso01-my.sharepoint.com/personal/santiago_ayon_iteso_mx/Documents/Santiago/ITESO/Semestre 2/Programacion para analisis de datos/Proyecto/Proyecto_prog_analisis/raw_data/raw_data_post_pan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15672806-3C23-4494-B37F-A01E28A9AE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{15672806-3C23-4494-B37F-A01E28A9AE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84485D0B-D3E4-4A5E-88E8-71E9281DAE1E}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{B4A5C79B-A43A-4CD1-BAC9-FB77BFD4D9B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{B4A5C79B-A43A-4CD1-BAC9-FB77BFD4D9B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Vista02" sheetId="1" r:id="rId1"/>
+    <sheet name="Alojamiento" sheetId="1" r:id="rId1"/>
     <sheet name="Vista03" sheetId="2" r:id="rId2"/>
     <sheet name="Vista04" sheetId="3" r:id="rId3"/>
     <sheet name="Vista05" sheetId="4" r:id="rId4"/>
@@ -486,19 +486,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B7BD8B-876C-4E69-B759-65062B881192}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -522,7 +522,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2013</v>
       </c>
@@ -548,7 +548,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -572,7 +572,7 @@
         <v>19525</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2014</v>
       </c>
@@ -598,7 +598,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -622,7 +622,7 @@
         <v>19933</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2015</v>
       </c>
@@ -648,7 +648,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
@@ -672,7 +672,7 @@
         <v>18746</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2016</v>
       </c>
@@ -698,7 +698,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -722,7 +722,7 @@
         <v>18620</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2017</v>
       </c>
@@ -748,7 +748,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -772,7 +772,7 @@
         <v>18244</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2018</v>
       </c>
@@ -798,7 +798,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -822,7 +822,7 @@
         <v>18244</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2019</v>
       </c>
@@ -848,7 +848,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
@@ -872,7 +872,7 @@
         <v>19427</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2020</v>
       </c>
@@ -898,7 +898,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>5</v>
@@ -922,7 +922,7 @@
         <v>22093</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2021</v>
       </c>
@@ -948,7 +948,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>5</v>
@@ -972,7 +972,7 @@
         <v>21606</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2022</v>
       </c>
@@ -998,7 +998,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>5</v>
@@ -1022,7 +1022,7 @@
         <v>21967</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>5</v>
@@ -1085,15 +1085,15 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2013</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1113,7 +1113,7 @@
         <v>8.819165888235618E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2014</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -1133,7 +1133,7 @@
         <v>8.6419753086419748E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2015</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -1153,7 +1153,7 @@
         <v>8.4040323385567425E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2016</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
@@ -1173,7 +1173,7 @@
         <v>8.7834953758596152E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2017</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>2</v>
@@ -1193,7 +1193,7 @@
         <v>9.2775526926753768E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2018</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>2</v>
@@ -1213,7 +1213,7 @@
         <v>9.0336879432624112E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2019</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>2205</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>2</v>
@@ -1233,7 +1233,7 @@
         <v>9.3041900502130889E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2020</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>2628</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>2</v>
@@ -1253,7 +1253,7 @@
         <v>0.10642692260964647</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2021</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>2</v>
@@ -1273,7 +1273,7 @@
         <v>0.10491647156858855</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2022</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>2739</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>2</v>
@@ -1293,7 +1293,7 @@
         <v>0.10742440287092599</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>2821</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>2</v>
@@ -1323,18 +1323,18 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2013</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>62215</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -1354,7 +1354,7 @@
         <v>9.2541083094351301E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2014</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>63284</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -1374,7 +1374,7 @@
         <v>9.1404504362671529E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2015</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>66079</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -1394,7 +1394,7 @@
         <v>8.9718836896072296E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2016</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>70987</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -1414,7 +1414,7 @@
         <v>9.2294590676539223E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2017</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>75422</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>14</v>
@@ -1434,7 +1434,7 @@
         <v>9.4917958927865781E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2018</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>75422</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -1454,7 +1454,7 @@
         <v>9.3325579093248859E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2019</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>76405</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>14</v>
@@ -1474,7 +1474,7 @@
         <v>9.1358461643316388E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2020</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>78533</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>14</v>
@@ -1494,7 +1494,7 @@
         <v>9.1977756592092536E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2021</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>78969</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>14</v>
@@ -1514,7 +1514,7 @@
         <v>9.1048599837662336E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2022</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>82066</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>14</v>
@@ -1534,7 +1534,7 @@
         <v>9.3148638740008768E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>82778</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>14</v>
@@ -1561,260 +1561,237 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD0DE54-F56E-4CB2-8310-90CE5D00DA95}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>2013</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
         <v>1605</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>2014</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
         <v>1617</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3">
+      <c r="C5" s="3">
         <v>7.4766355140186919E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>2015</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
         <v>1684</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="3">
+      <c r="C7" s="3">
         <v>4.1434755720470007E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>2016</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
         <v>1852</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3">
+      <c r="C9" s="3">
         <v>9.9762470308788598E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>2017</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
         <v>2038</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="3">
+      <c r="C11" s="3">
         <v>0.10043196544276457</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>2018</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2">
         <v>2038</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="3">
+      <c r="C13" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>2019</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
         <v>2205</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="3">
+      <c r="C15" s="3">
         <v>8.1943081452404323E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>2020</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2">
         <v>2628</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3">
+      <c r="C17" s="3">
         <v>0.19183673469387755</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>2021</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2">
         <v>2644</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="3">
+      <c r="C19" s="3">
         <v>6.0882800608828003E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>2022</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2">
         <v>2739</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="3">
+      <c r="C21" s="3">
         <v>3.59304084720121E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>2023</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="2">
         <v>2821</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="3">
+      <c r="C23" s="3">
         <v>2.9937933552391383E-2</v>
       </c>
     </row>
@@ -1831,9 +1808,9 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1845,7 +1822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>2013</v>
@@ -1857,7 +1834,7 @@
         <v>62215</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -1865,7 +1842,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>2014</v>
@@ -1877,7 +1854,7 @@
         <v>63284</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -1887,7 +1864,7 @@
         <v>1.7182351522944627E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>2015</v>
@@ -1899,7 +1876,7 @@
         <v>66079</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -1909,7 +1886,7 @@
         <v>4.4165981922760889E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>2016</v>
@@ -1921,7 +1898,7 @@
         <v>70987</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -1931,7 +1908,7 @@
         <v>7.4274731760468532E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>2017</v>
@@ -1943,7 +1920,7 @@
         <v>75422</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -1953,7 +1930,7 @@
         <v>6.2476228041754123E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>2018</v>
@@ -1965,7 +1942,7 @@
         <v>75422</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -1975,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>2019</v>
@@ -1987,7 +1964,7 @@
         <v>76405</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
@@ -1997,7 +1974,7 @@
         <v>1.3033332449417942E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>2020</v>
@@ -2009,7 +1986,7 @@
         <v>78533</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -2019,7 +1996,7 @@
         <v>2.7851580393953277E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>2021</v>
@@ -2031,7 +2008,7 @@
         <v>78969</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
@@ -2041,7 +2018,7 @@
         <v>5.5518062470553782E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>2022</v>
@@ -2053,7 +2030,7 @@
         <v>82066</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
@@ -2063,7 +2040,7 @@
         <v>3.9217920956324634E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>2023</v>
@@ -2075,7 +2052,7 @@
         <v>82778</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">

</xml_diff>